<commit_message>
For det meste resultater, + fixes paa runclassifier, og iteratrerunclassifier
</commit_message>
<xml_diff>
--- a/it200.xlsx
+++ b/it200.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Ordit</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Best Res</t>
+  </si>
+  <si>
+    <t>Regularization param found by cross validation</t>
+  </si>
+  <si>
+    <t>Regularization parm fixed</t>
   </si>
 </sst>
 </file>
@@ -81,8 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1076,68 +1085,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>0.41254125412499998</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>0.43036303630400002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>0.420462046205</v>
-      </c>
       <c r="D3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>0.43036303630400002</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>0.40594059405900002</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>0.41386138613899998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>0.43432343234300003</v>
+        <v>0.420462046205</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -1145,86 +1172,137 @@
       <c r="E4">
         <v>0.43036303630400002</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>0.40792079207900001</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>0.415181518152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>0.43432343234300003</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5">
+        <v>0.43036303630400002</v>
+      </c>
+      <c r="F5">
+        <v>0.41122112211200001</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>0.41584158415799999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0.43432343234300003</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
         <v>0.43693696370000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
+      <c r="F6">
+        <v>0.41320132013200001</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>0.41320132013200001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>0.86072607260699996</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
         <v>0.87128712871299996</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
+      <c r="F7">
+        <v>0.86336633663399998</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0.873267326733</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
         <v>0.86666666666600001</v>
       </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
         <v>0.873267326733</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
+      <c r="F8">
+        <v>0.87128712871299996</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>0.87722772277200001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
         <v>0.87524752475199996</v>
       </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <v>0.87524752475199996</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>0.87788778877899998</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>0.87788778877899998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>2</v>
-      </c>
+      <c r="F9">
+        <v>0.87854785478499997</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>0.87854785478499997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="B10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>0.87788778877899998</v>
@@ -1233,29 +1311,50 @@
         <v>4</v>
       </c>
       <c r="E10">
+        <v>0.87788778877899998</v>
+      </c>
+      <c r="F10">
+        <v>0.87920792079200005</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>0.87986798679900002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0.87788778877899998</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
         <v>0.89306930693099995</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
+      <c r="F11">
+        <v>0.88778877887800001</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>0.90363036303599997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
         <v>0.89306930693099995</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>0.90165016501700002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>0.89900990099</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -1263,190 +1362,307 @@
       <c r="E12">
         <v>0.90165016501700002</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>0.89306930693099995</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>0.90165016501700002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
+        <v>0.89900990099</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>0.90165016501700002</v>
+      </c>
+      <c r="F13">
+        <v>0.89768976897700004</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>0.90363036303599997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
         <v>0.89966996699699997</v>
       </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>0.89966996699699997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>0.88976897689800005</v>
-      </c>
       <c r="D14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>0.89966996699699997</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>0.90495049505000003</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>0.90495049505000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>3</v>
+      </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15">
+        <v>0.88976897689800005</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>0.89966996699699997</v>
+      </c>
+      <c r="F15">
+        <v>0.88976897689800005</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>0.89966996699699997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
         <v>0.89768976897700004</v>
       </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
         <v>0.90363036303599997</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
+      <c r="F16">
+        <v>0.90165016501700002</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>0.90759075907599995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
         <v>0.90363036303599997</v>
       </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16">
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
         <v>0.90561056105600002</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17">
+      <c r="F17">
+        <v>0.90627062706299999</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>0.90825082508300004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
         <v>0.91155115511600004</v>
       </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="E17">
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
         <v>0.91155115511600004</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
+      <c r="F18">
+        <v>0.91155115511600004</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>0.91155115511600004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>0.888448844884</v>
       </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
         <v>0.88910891089099997</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
+      <c r="F19">
+        <v>0.89570957095699999</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0.89570957095699999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
         <v>0.90297029702999998</v>
       </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19">
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
         <v>0.90693069306899998</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20">
+      <c r="F20">
+        <v>0.90297029702999998</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>0.90693069306899998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
         <v>0.90561056105600002</v>
       </c>
-      <c r="D20">
-        <v>4</v>
-      </c>
-      <c r="E20">
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
         <v>0.909570957096</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
+      <c r="F21">
+        <v>0.90561056105600002</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>0.909570957096</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
         <v>0.91023102310199999</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
         <v>0.91221122112200004</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
+      <c r="F22">
+        <v>0.91023102310199999</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0.91221122112200004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
         <v>5</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
         <v>0.88646864686500004</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
         <v>0.88646864686500004</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23">
+      <c r="F23">
+        <v>0.89900990099</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0.89900990099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
         <v>0.89636963696399996</v>
       </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23">
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
         <v>0.89636963696399996</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24">
+      <c r="F24">
+        <v>0.89900990099</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0.90891089108900003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
         <v>0.90363036303599997</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>0.91419141914199997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="C25">
-        <v>0.91023102310199999</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1454,55 +1670,91 @@
       <c r="E25">
         <v>0.91419141914199997</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
+      <c r="F25">
+        <v>0.90363036303599997</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0.91419141914199997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>0.91023102310199999</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0.91419141914199997</v>
+      </c>
+      <c r="F26">
+        <v>0.91023102310199999</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0.91419141914199997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
         <v>6</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
         <v>0.88778877887800001</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
         <v>0.88778877887800001</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27">
+      <c r="F27">
+        <v>0.89570957095699999</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0.89570957095699999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
         <v>0.90297029702999998</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
         <v>0.909570957096</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>0.90363036303599997</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>0.91617161716200002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <v>0.90627062706299999</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0.91485148514900005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="B29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>0.90363036303599997</v>
@@ -1511,69 +1763,141 @@
         <v>1</v>
       </c>
       <c r="E29">
+        <v>0.91617161716200002</v>
+      </c>
+      <c r="F29">
+        <v>0.90363036303599997</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0.91617161716200002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>0.90363036303599997</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
         <v>0.91815181518199995</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
+      <c r="F30">
+        <v>0.90363036303599997</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0.91815181518199995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
         <v>7</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
         <v>0.89306930693099995</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
         <v>0.89306930693099995</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
+      <c r="F31">
+        <v>0.90231023102300001</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0.90231023102300001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
         <v>0.90627062706299999</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
         <v>0.91485148514900005</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32">
+      <c r="F32">
+        <v>0.91089108910899996</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0.91881188118799995</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
         <v>0.90429042904300005</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
         <v>0.91617161716200002</v>
       </c>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33">
+      <c r="F33">
+        <v>0.90429042904300005</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>0.91617161716200002</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
         <v>0.89240924092399998</v>
       </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33">
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
         <v>0.90363036303599997</v>
       </c>
+      <c r="F34">
+        <v>0.90297029702999998</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>0.91287128712900001</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Sletter tidligere filer ved splitting
</commit_message>
<xml_diff>
--- a/it200.xlsx
+++ b/it200.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Ordit</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Regularization parm fixed</t>
+  </si>
+  <si>
+    <t>Dev avg file length:</t>
+  </si>
+  <si>
+    <t>Train avg file length:</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -386,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1061,7 +1070,7 @@
         <v>0.29126299999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="1:6">
       <c r="B33">
         <v>4</v>
       </c>
@@ -1076,6 +1085,28 @@
       </c>
       <c r="F33">
         <v>0.25339800000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>30.03</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>290.14</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1087,7 +1118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>

</xml_diff>